<commit_message>
add grouptag tag, for test plan
</commit_message>
<xml_diff>
--- a/testsheet.xlsx
+++ b/testsheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -46,6 +46,9 @@
     <t xml:space="preserve">encoded form where</t>
   </si>
   <si>
+    <t xml:space="preserve">grouptag</t>
+  </si>
+  <si>
     <t xml:space="preserve">time</t>
   </si>
   <si>
@@ -76,6 +79,9 @@
     <t xml:space="preserve">/home/cxh/Database/10_frames_0.5.yuv</t>
   </si>
   <si>
+    <t xml:space="preserve">hevc01</t>
+  </si>
+  <si>
     <t xml:space="preserve">10_frames_2.yuv</t>
   </si>
   <si>
@@ -98,6 +104,9 @@
   </si>
   <si>
     <t xml:space="preserve">/home/cxh/Database/10_frames_hevc_0.5.yuv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hevc02</t>
   </si>
   <si>
     <t xml:space="preserve">10_frames_hevc_2.yuv</t>
@@ -125,11 +134,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -147,117 +157,27 @@
       <family val="0"/>
     </font>
     <font>
+      <i val="true"/>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Lohit Devanagari"/>
+      <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF0000EE"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -265,23 +185,8 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -305,119 +210,29 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000EE"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -426,16 +241,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="K16" activeCellId="0" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="38.76"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="11.52"/>
@@ -471,74 +286,77 @@
       <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>4096</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>2106</v>
+        <v>2160</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>8</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>4096</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>2160</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="0" t="s">
         <v>14</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>4096</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>2106</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>4096</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>2106</v>
+        <v>2160</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>8</v>
@@ -547,24 +365,27 @@
         <v>500</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>4096</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>2106</v>
+        <v>2160</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>8</v>
@@ -573,24 +394,27 @@
         <v>2000</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>4096</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>2106</v>
+        <v>2160</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>8</v>
@@ -599,24 +423,27 @@
         <v>4500</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>4096</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>2106</v>
+        <v>2160</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>8</v>
@@ -625,24 +452,27 @@
         <v>13000</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>4096</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>2106</v>
+        <v>2160</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>8</v>
@@ -651,24 +481,27 @@
         <v>500</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>4096</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>2106</v>
+        <v>2160</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>8</v>
@@ -677,24 +510,27 @@
         <v>2000</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>4096</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>2106</v>
+        <v>2160</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>8</v>
@@ -703,24 +539,27 @@
         <v>4500</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>4096</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>2106</v>
+        <v>2160</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>8</v>
@@ -729,7 +568,10 @@
         <v>13000</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix 10bits bug, and add more plot show
</commit_message>
<xml_diff>
--- a/testsheet.xlsx
+++ b/testsheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="57">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -67,10 +67,10 @@
     <t xml:space="preserve">Original</t>
   </si>
   <si>
-    <t xml:space="preserve">10_hecv.yuv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/cxh/Database/10_hevc.yuv</t>
+    <t xml:space="preserve">10_frames_hevc_Origin.yuv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/cxh/Database/Database/10_frames_hevc_Origin.yuv</t>
   </si>
   <si>
     <t xml:space="preserve">10_frames_0.5.yuv</t>
@@ -100,31 +100,357 @@
     <t xml:space="preserve">/home/cxh/Database/10_frames_13.yuv</t>
   </si>
   <si>
-    <t xml:space="preserve">10_frames_hevc_0.5.yuv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/cxh/Database/10_frames_hevc_0.5.yuv</t>
+    <t xml:space="preserve">10_frames_hevc_0.5M.yuv</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/home/cxh/Database/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Database/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">10_frames_hevc_0.5M.yuv</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">hevc02</t>
   </si>
   <si>
-    <t xml:space="preserve">10_frames_hevc_2.yuv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/cxh/Database/10_frames_hevc_2.yuv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10_frames_hevc_4.5.yuv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/cxh/Database/10_frames_hevc_4.5.yuv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10_frames_hevc_13.yuv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/cxh/Database/10_frames_hevc_13.yuv</t>
+    <t xml:space="preserve">10_frames_hevc_2M.yuv</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/home/cxh/Database/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Database/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">10_frames_hevc_2M.yuv</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">10_frames_hevc_4.5M.yuv</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/home/cxh/Database/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Database/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">10_frames_hevc_4.5M.yuv</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">10_frames_hevc_13M.yuv</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/home/cxh/Database/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Database/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">10_frames_hevc_13M.yuv</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">10_frames_8k10hevc_0.5M.yuv</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/home/cxh/Database/Database/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">10_frames_8k10hevc_0.5M.yuv</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">10_frames_8k10hevc_Origin.yuv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8k10hevc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10_frames_8k10hevc_13M.yuv</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/home/cxh/Database/Database/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">10_frames_8k10hevc_13M.yuv</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">10_frames_8k10hevc_2M.yuv</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/home/cxh/Database/Database/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">10_frames_8k10hevc_2M.yuv</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">10_frames_8k10hevc_4.5M.yuv</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/home/cxh/Database/Database/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">10_frames_8k10hevc_4.5M.yuv</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/home/cxh/Database/Database/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">10_frames_8k10hevc_Origin.yuv</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">10to8_0.5.yuv</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/home/cxh/Database/Database/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">10to8_0.5.yuv</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">10to8_origin.yuv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8khevc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10to8_13.yuv</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/home/cxh/Database/Database/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">10to8_13.yuv</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">10to8_2.yuv</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/home/cxh/Database/Database/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">10to8_2.yuv</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">10to8_4.5.yuv</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/home/cxh/Database/Database/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">10to8_4.5.yuv</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/home/cxh/Database/Database/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">10to8_origin.yuv</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -220,7 +546,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -241,20 +567,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K16" activeCellId="0" sqref="K16"/>
+      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="38.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="58.22"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="27.37"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -572,6 +898,293 @@
       </c>
       <c r="I11" s="0" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>7680</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>3840</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>7680</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>3840</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>13000</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>7680</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>3840</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>7680</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>3840</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>4500</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>7680</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>3840</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>87610</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>7680</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>3840</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>9501</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>7680</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>3840</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>11752</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>7680</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>3840</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>9482</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>7680</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>3840</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>9073</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="I20" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>7680</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>3840</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>87610</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>